<commit_message>
fix and refactor lab2
</commit_message>
<xml_diff>
--- a/lab2/TT.xlsx
+++ b/lab2/TT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\sm_labs\lab2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobzev\Documents\GitHub\sm_labs\lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,36 +15,14 @@
     <sheet name="TT" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Database">TT!$A$1:$G$101</definedName>
+    <definedName name="_xlnm.Database">TT!$A$1:$G$100</definedName>
   </definedNames>
   <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>T6</t>
-  </si>
-  <si>
-    <t>TO</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection sqref="A1:A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -396,26 +374,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+      <c r="A1" s="1">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -423,45 +401,45 @@
         <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1">
-        <v>390</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1">
-        <v>183</v>
+        <v>628</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -469,160 +447,160 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
-        <v>628</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1">
-        <v>566</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F6" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G6" s="1">
-        <v>313</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1">
-        <v>90</v>
+        <v>549</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1">
         <v>4</v>
       </c>
       <c r="F8" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G8" s="1">
-        <v>549</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F9" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1">
-        <v>133</v>
+        <v>535</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" s="1">
-        <v>535</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -633,42 +611,42 @@
         <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="G11" s="1">
-        <v>422</v>
+        <v>556</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G12" s="1">
-        <v>556</v>
+        <v>588</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -676,91 +654,91 @@
         <v>5</v>
       </c>
       <c r="B13" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F13" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G13" s="1">
-        <v>588</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E14" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F14" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G14" s="1">
-        <v>267</v>
+        <v>419</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
         <v>6</v>
       </c>
       <c r="E15" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F15" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G15" s="1">
-        <v>419</v>
+        <v>530</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E16" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G16" s="1">
-        <v>530</v>
+        <v>546</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -768,114 +746,114 @@
         <v>10</v>
       </c>
       <c r="B17" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="1">
         <v>7</v>
       </c>
       <c r="E17" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F17" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G17" s="1">
-        <v>546</v>
+        <v>474</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E18" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F18" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G18" s="1">
-        <v>474</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E19" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F19" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G19" s="1">
-        <v>363</v>
+        <v>407</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
       </c>
       <c r="D20" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F20" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G20" s="1">
-        <v>407</v>
+        <v>400</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C21" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D21" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F21" s="1">
         <v>10</v>
       </c>
       <c r="G21" s="1">
-        <v>400</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -883,367 +861,367 @@
         <v>9</v>
       </c>
       <c r="B22" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F22" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G22" s="1">
-        <v>131</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B23" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D23" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E23" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G23" s="1">
-        <v>251</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E24" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F24" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G24" s="1">
-        <v>144</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B25" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C25" s="1">
         <v>4</v>
       </c>
       <c r="D25" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E25" s="1">
         <v>5</v>
       </c>
       <c r="F25" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G25" s="1">
-        <v>56</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B26" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D26" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E26" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F26" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G26" s="1">
-        <v>348</v>
+        <v>391</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B27" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C27" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E27" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F27" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G27" s="1">
-        <v>391</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B28" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C28" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D28" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E28" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F28" s="1">
         <v>7</v>
       </c>
       <c r="G28" s="1">
-        <v>291</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B29" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C29" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D29" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E29" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F29" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G29" s="1">
-        <v>270</v>
+        <v>408</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D30" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E30" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F30" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G30" s="1">
-        <v>408</v>
+        <v>373</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C31" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D31" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E31" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F31" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G31" s="1">
-        <v>373</v>
+        <v>489</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B32" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E32" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G32" s="1">
-        <v>489</v>
+        <v>532</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B33" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C33" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D33" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E33" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F33" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G33" s="1">
-        <v>532</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B34" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D34" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E34" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F34" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G34" s="1">
-        <v>221</v>
+        <v>282</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B35" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C35" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D35" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E35" s="1">
         <v>8</v>
       </c>
       <c r="F35" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G35" s="1">
-        <v>282</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B36" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C36" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D36" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E36" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F36" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G36" s="1">
-        <v>238</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B37" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C37" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E37" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F37" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G37" s="1">
-        <v>83</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1251,148 +1229,148 @@
         <v>7</v>
       </c>
       <c r="B38" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C38" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D38" s="1">
         <v>3</v>
       </c>
       <c r="E38" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F38" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G38" s="1">
-        <v>244</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B39" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C39" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D39" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E39" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F39" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G39" s="1">
-        <v>49</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B40" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C40" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D40" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E40" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G40" s="1">
-        <v>220</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B41" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C41" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D41" s="1">
         <v>5</v>
       </c>
       <c r="E41" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F41" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G41" s="1">
-        <v>171</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B42" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C42" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D42" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E42" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F42" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G42" s="1">
-        <v>147</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B43" s="1">
         <v>4</v>
       </c>
       <c r="C43" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D43" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E43" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F43" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G43" s="1">
-        <v>68</v>
+        <v>390</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B44" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D44" s="1">
         <v>10</v>
@@ -1401,67 +1379,67 @@
         <v>3</v>
       </c>
       <c r="F44" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G44" s="1">
-        <v>390</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B45" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C45" s="1">
         <v>1</v>
       </c>
       <c r="D45" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E45" s="1">
         <v>3</v>
       </c>
       <c r="F45" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G45" s="1">
-        <v>239</v>
+        <v>334</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B46" s="1">
         <v>5</v>
       </c>
       <c r="C46" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D46" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E46" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F46" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G46" s="1">
-        <v>334</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B47" s="1">
         <v>5</v>
       </c>
       <c r="C47" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D47" s="1">
         <v>10</v>
@@ -1470,286 +1448,286 @@
         <v>10</v>
       </c>
       <c r="F47" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G47" s="1">
-        <v>170</v>
+        <v>377</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B48" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C48" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D48" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E48" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F48" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G48" s="1">
-        <v>377</v>
+        <v>526</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B49" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C49" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D49" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E49" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F49" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G49" s="1">
-        <v>526</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B50" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C50" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D50" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E50" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F50" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G50" s="1">
-        <v>101</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B51" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C51" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D51" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E51" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F51" s="1">
         <v>6</v>
       </c>
       <c r="G51" s="1">
-        <v>59</v>
+        <v>600</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B52" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C52" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D52" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E52" s="1">
         <v>4</v>
       </c>
       <c r="F52" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G52" s="1">
-        <v>600</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B53" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C53" s="1">
         <v>5</v>
       </c>
       <c r="D53" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E53" s="1">
         <v>4</v>
       </c>
       <c r="F53" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G53" s="1">
-        <v>40</v>
+        <v>479</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B54" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C54" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D54" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E54" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F54" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G54" s="1">
-        <v>479</v>
+        <v>506</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B55" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C55" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D55" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F55" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G55" s="1">
-        <v>506</v>
+        <v>229</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B56" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C56" s="1">
         <v>4</v>
       </c>
       <c r="D56" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E56" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F56" s="1">
         <v>1</v>
       </c>
       <c r="G56" s="1">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B57" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C57" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D57" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E57" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F57" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G57" s="1">
-        <v>233</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B58" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C58" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D58" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E58" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F58" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G58" s="1">
-        <v>48</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B59" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C59" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D59" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E59" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F59" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G59" s="1">
-        <v>150</v>
+        <v>375</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -1757,45 +1735,45 @@
         <v>4</v>
       </c>
       <c r="B60" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C60" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D60" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E60" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F60" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G60" s="1">
-        <v>375</v>
+        <v>354</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B61" s="1">
         <v>2</v>
       </c>
       <c r="C61" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D61" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E61" s="1">
         <v>1</v>
       </c>
       <c r="F61" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G61" s="1">
-        <v>354</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -1803,45 +1781,45 @@
         <v>8</v>
       </c>
       <c r="B62" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C62" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D62" s="1">
         <v>4</v>
       </c>
       <c r="E62" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F62" s="1">
         <v>10</v>
       </c>
       <c r="G62" s="1">
-        <v>148</v>
+        <v>422</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B63" s="1">
         <v>4</v>
       </c>
       <c r="C63" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D63" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E63" s="1">
         <v>7</v>
       </c>
       <c r="F63" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G63" s="1">
-        <v>422</v>
+        <v>384</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -1849,160 +1827,160 @@
         <v>9</v>
       </c>
       <c r="B64" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C64" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D64" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E64" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G64" s="1">
-        <v>384</v>
+        <v>397</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B65" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C65" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D65" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E65" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F65" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G65" s="1">
-        <v>397</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B66" s="1">
         <v>10</v>
       </c>
       <c r="C66" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D66" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E66" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F66" s="1">
         <v>3</v>
       </c>
       <c r="G66" s="1">
-        <v>177</v>
+        <v>568</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B67" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C67" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D67" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E67" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F67" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G67" s="1">
-        <v>568</v>
+        <v>284</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B68" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C68" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D68" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E68" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F68" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G68" s="1">
-        <v>284</v>
+        <v>437</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B69" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C69" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D69" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E69" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F69" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G69" s="1">
-        <v>437</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B70" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C70" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D70" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E70" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F70" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G70" s="1">
-        <v>126</v>
+        <v>511</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -2010,335 +1988,335 @@
         <v>4</v>
       </c>
       <c r="B71" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C71" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D71" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E71" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F71" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G71" s="1">
-        <v>511</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B72" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C72" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D72" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E72" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G72" s="1">
-        <v>64</v>
+        <v>511</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B73" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C73" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D73" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E73" s="1">
         <v>1</v>
       </c>
       <c r="F73" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G73" s="1">
-        <v>511</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B74" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C74" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D74" s="1">
         <v>1</v>
       </c>
       <c r="E74" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F74" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G74" s="1">
-        <v>126</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B75" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C75" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D75" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E75" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F75" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G75" s="1">
-        <v>232</v>
+        <v>359</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B76" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C76" s="1">
         <v>6</v>
       </c>
       <c r="D76" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E76" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F76" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G76" s="1">
-        <v>359</v>
+        <v>304</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B77" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C77" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D77" s="1">
         <v>1</v>
       </c>
       <c r="E77" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F77" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G77" s="1">
-        <v>304</v>
+        <v>569</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B78" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C78" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D78" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E78" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F78" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G78" s="1">
-        <v>569</v>
+        <v>392</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B79" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C79" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D79" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E79" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F79" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G79" s="1">
-        <v>392</v>
+        <v>536</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B80" s="1">
         <v>6</v>
       </c>
       <c r="C80" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D80" s="1">
         <v>9</v>
       </c>
       <c r="E80" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F80" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G80" s="1">
-        <v>536</v>
+        <v>324</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B81" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C81" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D81" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E81" s="1">
         <v>2</v>
       </c>
       <c r="F81" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G81" s="1">
-        <v>324</v>
+        <v>516</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B82" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C82" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D82" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E82" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F82" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G82" s="1">
-        <v>516</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B83" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C83" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D83" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E83" s="1">
         <v>4</v>
       </c>
       <c r="F83" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G83" s="1">
-        <v>225</v>
+        <v>187</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B84" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C84" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D84" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E84" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F84" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G84" s="1">
-        <v>187</v>
+        <v>482</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B85" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C85" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D85" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E85" s="1">
         <v>6</v>
@@ -2347,340 +2325,340 @@
         <v>9</v>
       </c>
       <c r="G85" s="1">
-        <v>482</v>
+        <v>242</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B86" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C86" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D86" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E86" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F86" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G86" s="1">
-        <v>242</v>
+        <v>206</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B87" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C87" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D87" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E87" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F87" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G87" s="1">
-        <v>206</v>
+        <v>390</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B88" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C88" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D88" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E88" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F88" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G88" s="1">
-        <v>390</v>
+        <v>482</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B89" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D89" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E89" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F89" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G89" s="1">
-        <v>482</v>
+        <v>286</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B90" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C90" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D90" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E90" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F90" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G90" s="1">
-        <v>286</v>
+        <v>318</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B91" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C91" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D91" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E91" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F91" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G91" s="1">
-        <v>318</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B92" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C92" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D92" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E92" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F92" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G92" s="1">
-        <v>130</v>
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B93" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C93" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D93" s="1">
         <v>10</v>
       </c>
       <c r="E93" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F93" s="1">
         <v>4</v>
       </c>
       <c r="G93" s="1">
-        <v>215</v>
+        <v>483</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B94" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C94" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D94" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E94" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F94" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G94" s="1">
-        <v>483</v>
+        <v>373</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B95" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C95" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D95" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E95" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F95" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G95" s="1">
-        <v>373</v>
+        <v>423</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B96" s="1">
         <v>4</v>
       </c>
       <c r="C96" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D96" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E96" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F96" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G96" s="1">
-        <v>423</v>
+        <v>34</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B97" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C97" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D97" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E97" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F97" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G97" s="1">
-        <v>34</v>
+        <v>198</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B98" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C98" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D98" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E98" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F98" s="1">
         <v>7</v>
       </c>
       <c r="G98" s="1">
-        <v>198</v>
+        <v>542</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B99" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C99" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D99" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E99" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F99" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G99" s="1">
-        <v>542</v>
+        <v>204</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B100" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C100" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D100" s="1">
         <v>10</v>
@@ -2689,32 +2667,9 @@
         <v>8</v>
       </c>
       <c r="F100" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G100" s="1">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="1">
-        <v>7</v>
-      </c>
-      <c r="B101" s="1">
-        <v>4</v>
-      </c>
-      <c r="C101" s="1">
-        <v>10</v>
-      </c>
-      <c r="D101" s="1">
-        <v>10</v>
-      </c>
-      <c r="E101" s="1">
-        <v>8</v>
-      </c>
-      <c r="F101" s="1">
-        <v>3</v>
-      </c>
-      <c r="G101" s="1">
         <v>309</v>
       </c>
     </row>

</xml_diff>